<commit_message>
Update DesignatedColors and upgrade plotting to use DesignatedColors
</commit_message>
<xml_diff>
--- a/src/Python/ddosi/plotting/Colors.xlsx
+++ b/src/Python/ddosi/plotting/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Research Post Processor\src\Python\ddosi\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E19342-F5F1-4CF2-A579-091E70666CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3522DA-6209-4CAC-B5B5-4339BCACF6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="-120" windowWidth="28020" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Acceleration X</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>#00FFFF</t>
+  </si>
+  <si>
+    <t>#9acd32</t>
+  </si>
+  <si>
+    <t>#ffd700</t>
+  </si>
+  <si>
+    <t>#f08080</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1073,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,9 +1100,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1101,9 +1112,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,9 +1124,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update the color list and add comments to DesignatedColors.
</commit_message>
<xml_diff>
--- a/src/Python/ddosi/plotting/Colors.xlsx
+++ b/src/Python/ddosi/plotting/Colors.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Research Post Processor\src\Python\ddosi\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551211C2-FAF7-456A-B95A-F6154F33F3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4295647B-61DA-4EB5-A7CB-7C4BAD78BADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="-120" windowWidth="28020" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="3855" windowWidth="20835" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Colors2" sheetId="1" r:id="rId1"/>
+    <sheet name="Colors" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Acceleration X</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>#8f99fb</t>
+  </si>
+  <si>
+    <t>Rate of Penetration</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -530,6 +533,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -575,7 +591,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -585,6 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -633,17 +650,25 @@
   <dxfs count="6">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -765,7 +790,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:D9" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:D10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="4" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="2"/>
@@ -777,9 +802,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -817,7 +842,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -923,7 +948,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1065,7 +1090,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1073,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,36 +1182,46 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+      <c r="A7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>